<commit_message>
A Question was added to the SIQ sheet by Moustafa Ghareeb Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5800EDD4-FF7C-4128-89B4-F0D52086852B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F740EE-E0AF-4BA0-849C-3563233E1E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7C6C0B2-95F0-4571-A456-993A77695EB1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calling the ELEV is done by Up/Down switches </t>
+  </si>
+  <si>
+    <t>How many floors are there?</t>
+  </si>
+  <si>
+    <t>Floors number doesn't matter, because the motor will simulate the direction without the need for any counting</t>
+  </si>
+  <si>
+    <t>22/1/2020</t>
+  </si>
+  <si>
+    <t>24/1/2020</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -148,13 +166,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -473,17 +491,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C882A9-F419-4B39-ACE5-0CE3C7D7335C}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -493,14 +511,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -535,138 +553,150 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
new question added Signed-off-by: Donia102950 <donia1995mohamed@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F740EE-E0AF-4BA0-849C-3563233E1E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7C6C0B2-95F0-4571-A456-993A77695EB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ_Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -82,12 +76,27 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can access the elevator by his username and password </t>
+  </si>
+  <si>
+    <t>we can use keypad and each number in keypad has array of few character  as nokia mobile 6630</t>
+  </si>
+  <si>
+    <t>how can user enter his username?</t>
+  </si>
+  <si>
+    <t>elevator has lock system so must enter userID to access elevator</t>
+  </si>
+  <si>
+    <t>not answered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -287,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -481,18 +490,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C882A9-F419-4B39-ACE5-0CE3C7D7335C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,19 +585,37 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
SIQ modification by Donia Mohamed Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F740EE-E0AF-4BA0-849C-3563233E1E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B7C6C0B2-95F0-4571-A456-993A77695EB1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ_Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -82,12 +76,27 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can access the elevator by his username and password </t>
+  </si>
+  <si>
+    <t>we can use keypad and each number in keypad has array of few character  as nokia mobile 6630</t>
+  </si>
+  <si>
+    <t>how can user enter his username?</t>
+  </si>
+  <si>
+    <t>elevator has lock system so must enter userID to access elevator</t>
+  </si>
+  <si>
+    <t>not answered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -235,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -287,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -481,18 +490,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C882A9-F419-4B39-ACE5-0CE3C7D7335C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,19 +585,37 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="H4" s="4"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
Updated the CYRS document and the SIQ sheet Signed-off-by: Donia102950 <donia1995mohamed@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -78,19 +78,19 @@
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">user can access the elevator by his username and password </t>
-  </si>
-  <si>
-    <t>we can use keypad and each number in keypad has array of few character  as nokia mobile 6630</t>
-  </si>
-  <si>
-    <t>how can user enter his username?</t>
-  </si>
-  <si>
-    <t>elevator has lock system so must enter userID to access elevator</t>
-  </si>
-  <si>
-    <t>not answered</t>
+    <t xml:space="preserve">User can access the elevator by his username and password </t>
+  </si>
+  <si>
+    <t>Elevator has lock system so must enter userID to access elevator</t>
+  </si>
+  <si>
+    <t>How can user enter his username?</t>
+  </si>
+  <si>
+    <t>We can use keypad and each number in keypad has array of few character  as nokia mobile 6630</t>
+  </si>
+  <si>
+    <t>Not answered</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,21 +501,21 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="47.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -597,13 +597,13 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updated SRS version 1 according to changes in CYRS doc.
Updated SRS version 1 according to changes in CYRS doc. and adding new questions in SIQ sheet.
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Islam El-Bahnasawy\Documents\GitHub\Digital_Elevator\Input Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0418E4E-DF8F-4014-9F83-1F17098FADE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ_Sheet" sheetId="1" r:id="rId1"/>
@@ -14,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -91,13 +91,41 @@
   </si>
   <si>
     <t>Not answered</t>
+  </si>
+  <si>
+    <t>Req_AKRAM_CYRS_300_V1.0</t>
+  </si>
+  <si>
+    <t>{
+This requirement describe the behavior of elevator when the user enter ID correct 
+1) When pass the given ID correct the LCD will display OK 
+2) He can access the elevator by using two buttons up/down
+}</t>
+  </si>
+  <si>
+    <t>how many floors in the building? Is it fixed or not?</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Req_AKRAM_CYRS_500_V1.0</t>
+  </si>
+  <si>
+    <t>{
+	This requirement describe the reset functionality 
+A reset for whole system is done when pressing on/off button for 2 sec
+}</t>
+  </si>
+  <si>
+    <t>What is the reset State?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +155,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -167,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +218,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,36 +537,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="59.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="59.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.3">
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
@@ -529,7 +576,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -561,7 +608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -589,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -617,31 +664,59 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
+    <row r="5" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="7">
+        <v>43852</v>
+      </c>
+      <c r="G5" s="8">
+        <v>43853</v>
+      </c>
       <c r="H5" s="4"/>
       <c r="I5" s="3"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="7">
+        <v>43852</v>
+      </c>
+      <c r="G6" s="8">
+        <v>43853</v>
+      </c>
       <c r="H6" s="4"/>
       <c r="I6" s="3"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
@@ -653,7 +728,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
@@ -665,7 +740,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
@@ -677,7 +752,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
@@ -689,7 +764,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -701,7 +776,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -713,7 +788,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="3"/>

</xml_diff>

<commit_message>
Update SIQ sheet with Answers
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Islam El-Bahnasawy\Documents\GitHub\Digital_Elevator\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsharaby\Documents\GitHub\DELV_Mostafa\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0418E4E-DF8F-4014-9F83-1F17098FADE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ_Sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -64,9 +63,6 @@
   </si>
   <si>
     <t>How many floors are there?</t>
-  </si>
-  <si>
-    <t>Floors number doesn't matter, because the motor will simulate the direction without the need for any counting</t>
   </si>
   <si>
     <t>22/1/2020</t>
@@ -120,11 +116,27 @@
   <si>
     <t>What is the reset State?</t>
   </si>
+  <si>
+    <t xml:space="preserve">Floors number doesn't matter, because the motor will simulate the direction without the need for any counting </t>
+  </si>
+  <si>
+    <t>TSH: 23/01/2020 : I agree with this we just need simulation for up and down movement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 23/01/2020 : Yes you should have a Keypad for input , it is great idea to have each key can navigate some characteres </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 23/01/2020 : As we agreed doesn't matter how many floors then if the pass is ok then motor moves up / or down 
+as per the user request </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSH: 23/01/2020 : The reset here means that the system shall start as if it the first time , reset all user names and passords and all start all over again </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -215,22 +227,28 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,20 +579,20 @@
     <col min="6" max="6" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="118.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -608,7 +626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -616,24 +634,26 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="11" t="s">
+        <v>29</v>
+      </c>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -641,27 +661,29 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
@@ -669,25 +691,27 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>43852</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>43853</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
+      <c r="I5" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
@@ -695,25 +719,27 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>28</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="7">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6">
         <v>43852</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>43853</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updating the PP after the approval of the HSI Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsharaby\Documents\GitHub\DELV_Mostafa\Input Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AAEC1B-02D1-4D2B-8ADA-F4060AA4EFBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ_Sheet" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Digital Elevator_SIQ_Sheet</t>
   </si>
@@ -65,6 +66,9 @@
     <t>How many floors are there?</t>
   </si>
   <si>
+    <t>Floors number doesn't matter, because the motor will simulate the direction without the need for any counting</t>
+  </si>
+  <si>
     <t>22/1/2020</t>
   </si>
   <si>
@@ -89,55 +93,26 @@
     <t>Not answered</t>
   </si>
   <si>
-    <t>Req_AKRAM_CYRS_300_V1.0</t>
-  </si>
-  <si>
-    <t>{
-This requirement describe the behavior of elevator when the user enter ID correct 
-1) When pass the given ID correct the LCD will display OK 
-2) He can access the elevator by using two buttons up/down
-}</t>
-  </si>
-  <si>
-    <t>how many floors in the building? Is it fixed or not?</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Req_AKRAM_CYRS_500_V1.0</t>
-  </si>
-  <si>
-    <t>{
+    <t>What is the reset State?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 	This requirement describe the reset functionality 
 A reset for whole system is done when pressing on/off button for 2 sec
-}</t>
-  </si>
-  <si>
-    <t>What is the reset State?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Floors number doesn't matter, because the motor will simulate the direction without the need for any counting </t>
-  </si>
-  <si>
-    <t>TSH: 23/01/2020 : I agree with this we just need simulation for up and down movement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSH: 23/01/2020 : Yes you should have a Keypad for input , it is great idea to have each key can navigate some characteres </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSH: 23/01/2020 : As we agreed doesn't matter how many floors then if the pass is ok then motor moves up / or down 
-as per the user request </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TSH: 23/01/2020 : The reset here means that the system shall start as if it the first time , reset all user names and passords and all start all over again </t>
+</t>
+  </si>
+  <si>
+    <t>Req _ DIGELV _CYRS_05_V1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,12 +142,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -213,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -236,18 +205,11 @@
     <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -309,7 +271,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -361,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -562,39 +524,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="59.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="59.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="106.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="118.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="106.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -626,7 +588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -634,73 +596,69 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="I4" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="93.6" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F5" s="6">
         <v>43852</v>
@@ -709,40 +667,22 @@
         <v>43853</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="6">
-        <v>43852</v>
-      </c>
-      <c r="G6" s="7">
-        <v>43853</v>
-      </c>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="12" t="s">
-        <v>32</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
@@ -754,7 +694,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
@@ -766,7 +706,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
@@ -778,7 +718,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
@@ -790,7 +730,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -802,7 +742,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
@@ -814,18 +754,6 @@
       <c r="I12" s="3"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H1"/>

</xml_diff>

<commit_message>
Updated all the documents with the new company's logo Signed-off-by: Moustafa Ghareeb <moustafa.ghareeb.hpg@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/SIQ_Sheet.xlsx
+++ b/Input Documents/SIQ_Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moustafa Ghareeb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Digital_Elevator\Input Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F599D8-4017-45E3-B5B6-574D7C036B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37535AB6-91B0-4A3D-83A5-69A62C9BCDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,10 +215,10 @@
     <xf numFmtId="15" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -236,6 +236,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1171576</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2486026</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7026B58A-52F9-45EC-9E84-68C046028813}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1781176" y="19050"/>
+          <a:ext cx="1314450" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -281,7 +339,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -333,7 +391,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -538,7 +596,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,14 +615,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -672,7 +730,7 @@
       <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -784,5 +842,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>